<commit_message>
Transformer 연결시 issue 추가
</commit_message>
<xml_diff>
--- a/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -287,11 +287,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Vol으로 Pulse On time 조절시 allways On시 동작하지 않음
- - Halt 발생 : OP_LED control이 안됨</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>전원 ON시 buzzer 동작하지 않음 - 기능 미구현 상태</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -302,6 +297,68 @@
   <si>
     <t>Plasma On시 buzzer는 동작하나 동작중 Key Off시 buzzer가 Off되지 않고 끝까지 동작함
  - Key interrupt 발생시 바로 Off되도록 구현 필요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB 연결 및 제거시 buzzer 동작함
+ - USB 연결시에는 buzzer 동작이 없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vol으로 Pulse On time 조절시 allways On시 동작하지 않음
+ - Halt 발생 : OP_LED control이 안됨
+ - 12/30 S/W : Max에서 allways Off 상태가 됨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getPlasmaVolLevel()에서 if(ontime &lt; PLASMA_SPAN_TIME_PWM_MSEC) 조건에 따른 변수값 설정 부분 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Buzzer 동작중 KEY_OP_Pin interrupt 발생시 Buzzer OFF되도록 수정
+mc.c에 sendtoBuzzerOffCmd(); 추가
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mc.c의 MC_EXTPWR_IN_EVT/ MC_EXTPWR_OUT_EVT case의 sendtoBuzzerOnCmd(2); 주석 처리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mc.c mctask_init() 함수에 sendtoBuzzerOnCmd(2); 추가
+ - Power On시 buzzer2 On 시킴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM1 pulse off 상태에서 전압이 불안정함
+ - 정확히 0V가 아니라 0V 상태에서 흔들림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer 연결시 Pulse On 상태에서 Booster 전압이 흔들림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pulse Always on 상태에서 Battery 전압이 OFF 됨
+ - current 증가로 인한 short로 인식하는것으로 보임
+ - Battery를 제거 후 다시 연결해야 함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pulse Off 구간 시작 부분에서 Booster 전압이 흔들림 더 심함
+ - PWM이 off될때 High상태에서 천천히 떨어지기 때문에 생기는 문제임</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -620,20 +677,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -652,39 +700,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -700,7 +715,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -767,18 +781,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -789,6 +794,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1097,496 +1132,555 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.375" customWidth="1"/>
-    <col min="8" max="8" width="65.125" customWidth="1"/>
-    <col min="9" max="9" width="48.25" customWidth="1"/>
+    <col min="1" max="2" width="9" style="8"/>
+    <col min="3" max="3" width="11.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="8"/>
+    <col min="6" max="6" width="11.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="65.125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="48.25" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="42" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="9">
         <v>43086</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="45"/>
     </row>
     <row r="5" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="10">
         <v>43087</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="15" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="47">
+      <c r="B6" s="32">
         <v>3</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="33">
         <v>43090</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="33">
         <v>43090</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="52"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="47">
+      <c r="B7" s="32">
         <v>4</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="33">
         <v>43090</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="33">
         <v>43091</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="52"/>
-    </row>
-    <row r="8" spans="2:9" s="22" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="47">
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="32">
         <v>5</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="33">
         <v>43091</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="33">
         <v>43091</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="H8" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="37" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="22" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+    <row r="9" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="32">
         <v>6</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="33">
         <v>43091</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="33">
         <v>43091</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="32">
         <v>7</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="33">
         <v>43098</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="33">
+        <v>43099</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="32">
+        <v>8</v>
+      </c>
+      <c r="C11" s="33">
+        <v>43099</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="33">
+        <v>43099</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43099</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="7">
-        <v>8</v>
-      </c>
-      <c r="C11" s="24">
+      <c r="F12" s="10"/>
+      <c r="G12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="32">
+        <v>10</v>
+      </c>
+      <c r="C13" s="33">
         <v>43099</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D13" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="7">
-        <v>9</v>
-      </c>
-      <c r="C12" s="24">
+      <c r="E13" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="33">
         <v>43099</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="G13" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="37"/>
+    </row>
+    <row r="14" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B14" s="32">
+        <v>11</v>
+      </c>
+      <c r="C14" s="33">
+        <v>43099</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
-        <v>10</v>
-      </c>
-      <c r="C13" s="24">
+      <c r="E14" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="33">
         <v>43099</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="15" t="s">
+      <c r="G14" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="7">
-        <v>11</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="7">
+      <c r="H14" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B15" s="4">
         <v>12</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
+      <c r="C15" s="10">
+        <v>43099</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>13</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="7">
+      <c r="C16" s="10">
+        <v>43099</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="39"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B17" s="4">
         <v>14</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="7">
+      <c r="C17" s="10">
+        <v>43099</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="4">
         <v>15</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
+      <c r="C18" s="10">
+        <v>43099</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="39"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>16</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>17</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>18</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="7">
+      <c r="B22" s="4">
         <v>19</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="7">
+      <c r="B23" s="4">
         <v>20</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="7">
+      <c r="B24" s="4">
         <v>21</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
+      <c r="B25" s="4">
         <v>22</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="7">
+      <c r="B26" s="4">
         <v>23</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="7">
+      <c r="B27" s="4">
         <v>24</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>25</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="7">
+      <c r="B29" s="4">
         <v>26</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="7">
+      <c r="B30" s="4">
         <v>27</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="9">
+      <c r="B31" s="6">
         <v>28</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="20"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1605,470 +1699,470 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="22" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="47" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="22"/>
-    <col min="7" max="8" width="26.375" style="22" customWidth="1"/>
-    <col min="9" max="9" width="42.375" style="22" customWidth="1"/>
-    <col min="10" max="10" width="23.875" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="22"/>
+    <col min="1" max="1" width="4.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="47" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="8"/>
+    <col min="7" max="8" width="26.375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="42.375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="23.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="34">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="9">
         <v>43086</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="38">
+      <c r="B5" s="23">
         <v>2</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="10">
         <v>43086</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="38">
+      <c r="B6" s="23">
         <v>3</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="10">
         <v>43089</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="39" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="41"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="38">
+      <c r="B7" s="23">
         <v>4</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="10">
         <v>43091</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="41"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="38">
+      <c r="B8" s="23">
         <v>5</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="10">
         <v>43091</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="41"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="38">
+      <c r="B9" s="23">
         <v>6</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="41"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="38">
+      <c r="B10" s="23">
         <v>7</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="41"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="38">
+      <c r="B11" s="23">
         <v>8</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="41"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="38">
+      <c r="B12" s="23">
         <v>9</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="41"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="26"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="38">
+      <c r="B13" s="23">
         <v>10</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="41"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
+      <c r="B14" s="23">
         <v>11</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="41"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="26"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="38">
+      <c r="B15" s="23">
         <v>12</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="41"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="41"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="41"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="38"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="41"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="41"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="38"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="41"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="41"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="38"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="41"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="38"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="41"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="38"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="41"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="38"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="41"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="38"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="41"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="38"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="41"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="26"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="38"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="41"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="38"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="41"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="38"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="41"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="38"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="41"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="38"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="41"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="26"/>
     </row>
     <row r="33" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="44"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="46"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
TIM1 PWR issue 추가
</commit_message>
<xml_diff>
--- a/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -347,18 +347,33 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Transformer 연결시 Pulse On 상태에서 Booster 전압이 흔들림</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pulse Always on 상태에서 Battery 전압이 OFF 됨
+    <t>Pulse Off 구간 시작 부분에서 Booster 전압이 흔들림 더 심함
+ - PWM이 off될때 High상태에서 천천히 떨어지기 때문에 생기는 문제임</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PULSE_OUT1_Pin|PULSE_OUT2_Pin
+ - GPIO_PULLDOWN으로 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pulse Always On 상태에서도 Off 구간이 발생
+ - Off 구간 : 31.56usec</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer 연결시 Pulse Always on 상태에서 Battery 전압이 OFF 됨
  - current 증가로 인한 short로 인식하는것으로 보임
  - Battery를 제거 후 다시 연결해야 함</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Pulse Off 구간 시작 부분에서 Booster 전압이 흔들림 더 심함
- - PWM이 off될때 High상태에서 천천히 떨어지기 때문에 생기는 문제임</t>
+    <t>Transformer 연결시 Pulse On 상태에서 Booster 전압이 흔들림
+ - Pulse duty를 줄이고, switch 구간에 gap을 추가하면 개선됨</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -677,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,6 +839,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1132,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1442,26 +1475,30 @@
       <c r="I14" s="37"/>
     </row>
     <row r="15" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="4">
+      <c r="B15" s="32">
         <v>12</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="33">
         <v>43099</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="28" t="s">
+      <c r="E15" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="33">
+        <v>43100</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>13</v>
       </c>
@@ -1476,30 +1513,32 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H16" s="39"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B17" s="4">
+      <c r="B17" s="50">
         <v>14</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="51">
         <v>43099</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="28" t="s">
+      <c r="D17" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="12"/>
+      <c r="E17" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="51">
+        <v>43100</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
     </row>
     <row r="18" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
@@ -1516,20 +1555,28 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>16</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="10">
+        <v>43100</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="28"/>
+      <c r="G19" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="H19" s="39"/>
       <c r="I19" s="12"/>
     </row>

</xml_diff>

<commit_message>
Volume 180deg 회전  - 이에 따른 RESET Key 위치 변경
</commit_message>
<xml_diff>
--- a/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
+++ b/V2.0/Plasma_Gen_Issue and ECO list_20171218.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="Issue list" sheetId="1" r:id="rId1"/>
     <sheet name="ECO list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,11 +170,6 @@
   </si>
   <si>
     <t>PIN이 아래쪽 방향</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCB 부품을 180도 회전시켜야 함
- - Knob의 방향이 반대방향으로 회전함</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -454,6 +449,35 @@
   </si>
   <si>
     <t>PCB Library 수정
+Plasma_Gen_Main Board_PCB_V1.0_20180102.pcb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB 부품을 180도 회전
+ - Knob의 방향이 반대방향으로 회전함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PCB 수정
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ME Screw center 수정 필요</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_Main Board_SCH_V2.0_20180102.sch
 Plasma_Gen_Main Board_PCB_V1.0_20180102.pcb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -538,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -778,11 +802,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -856,9 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -889,9 +988,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -933,6 +1029,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,7 +1126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1029,7 +1161,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1241,7 +1373,7 @@
   <dimension ref="B1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1266,7 +1398,7 @@
     </row>
     <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1279,213 +1411,213 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B4" s="45">
+      <c r="B4" s="43">
         <v>1</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="44">
         <v>43086</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="44">
+        <v>43102</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="48"/>
+    </row>
+    <row r="5" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="29">
+        <v>2</v>
+      </c>
+      <c r="C5" s="30">
+        <v>43087</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="30">
+        <v>43102</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="29">
+        <v>3</v>
+      </c>
+      <c r="C6" s="30">
+        <v>43090</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="30">
+        <v>43090</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B7" s="29">
+        <v>4</v>
+      </c>
+      <c r="C7" s="30">
+        <v>43090</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="46">
-        <v>43102</v>
-      </c>
-      <c r="G4" s="48" t="s">
+      <c r="E7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="30">
+        <v>43091</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="29">
+        <v>5</v>
+      </c>
+      <c r="C8" s="30">
+        <v>43091</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="30">
+        <v>43091</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="29">
+        <v>6</v>
+      </c>
+      <c r="C9" s="30">
+        <v>43091</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="30">
+        <v>43091</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="29">
+        <v>7</v>
+      </c>
+      <c r="C10" s="30">
+        <v>43098</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="30">
+        <v>43099</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="29">
         <v>8</v>
       </c>
-      <c r="H4" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="50"/>
-    </row>
-    <row r="5" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="30">
-        <v>2</v>
-      </c>
-      <c r="C5" s="31">
-        <v>43087</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="31">
-        <v>43102</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="30">
-        <v>3</v>
-      </c>
-      <c r="C6" s="31">
-        <v>43090</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="31">
-        <v>43090</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="35"/>
-    </row>
-    <row r="7" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="30">
-        <v>4</v>
-      </c>
-      <c r="C7" s="31">
-        <v>43090</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="31">
-        <v>43091</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="35"/>
-    </row>
-    <row r="8" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="30">
-        <v>5</v>
-      </c>
-      <c r="C8" s="31">
-        <v>43091</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="31">
-        <v>43091</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="30">
-        <v>6</v>
-      </c>
-      <c r="C9" s="31">
-        <v>43091</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="31">
-        <v>43091</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="33" t="s">
+      <c r="C11" s="30">
+        <v>43099</v>
+      </c>
+      <c r="D11" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="30">
-        <v>7</v>
-      </c>
-      <c r="C10" s="31">
-        <v>43098</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="31">
+      <c r="E11" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="30">
         <v>43099</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="30">
-        <v>8</v>
-      </c>
-      <c r="C11" s="31">
-        <v>43099</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="31">
-        <v>43099</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="35"/>
+      <c r="G11" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
@@ -1495,89 +1627,89 @@
         <v>43099</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="35"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="29">
+        <v>10</v>
+      </c>
+      <c r="C13" s="30">
+        <v>43099</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="30">
+        <v>43099</v>
+      </c>
+      <c r="G13" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="30">
-        <v>10</v>
-      </c>
-      <c r="C13" s="31">
+      <c r="H13" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B14" s="29">
+        <v>11</v>
+      </c>
+      <c r="C14" s="30">
         <v>43099</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="31">
+      <c r="D14" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="30">
         <v>43099</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G14" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H14" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B14" s="30">
-        <v>11</v>
-      </c>
-      <c r="C14" s="31">
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B15" s="29">
+        <v>12</v>
+      </c>
+      <c r="C15" s="30">
         <v>43099</v>
       </c>
-      <c r="D14" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="31">
-        <v>43099</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="30">
-        <v>12</v>
-      </c>
-      <c r="C15" s="31">
-        <v>43099</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="31">
+      <c r="D15" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="30">
         <v>43100</v>
       </c>
-      <c r="G15" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="35"/>
+      <c r="G15" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="2:9" ht="66" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
@@ -1587,91 +1719,91 @@
         <v>43099</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="2:9" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="29">
+        <v>14</v>
+      </c>
+      <c r="C17" s="30">
+        <v>43099</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" s="37" t="s">
+      <c r="E17" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="30">
+        <v>43102</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="34"/>
+    </row>
+    <row r="18" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="29">
+        <v>15</v>
+      </c>
+      <c r="C18" s="30">
+        <v>43099</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="30">
+        <v>43102</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="2:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="29">
+        <v>16</v>
+      </c>
+      <c r="C19" s="30">
+        <v>43100</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="30">
+        <v>43102</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="2:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="30">
-        <v>14</v>
-      </c>
-      <c r="C17" s="31">
-        <v>43099</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="31">
-        <v>43102</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="30">
-        <v>15</v>
-      </c>
-      <c r="C18" s="31">
-        <v>43099</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="31">
-        <v>43102</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B19" s="30">
-        <v>16</v>
-      </c>
-      <c r="C19" s="31">
-        <v>43100</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="31">
-        <v>43102</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="35"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
@@ -1681,8 +1813,8 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="37"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
@@ -1693,8 +1825,8 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="37"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1705,8 +1837,8 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
@@ -1717,8 +1849,8 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="37"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="35"/>
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
@@ -1729,8 +1861,8 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="37"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
@@ -1741,8 +1873,8 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="37"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
@@ -1753,8 +1885,8 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="37"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1765,8 +1897,8 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="37"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="35"/>
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1777,8 +1909,8 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="37"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1789,8 +1921,8 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="37"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="35"/>
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
@@ -1801,8 +1933,8 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="37"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="35"/>
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1813,14 +1945,14 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1834,20 +1966,20 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="6" customWidth="1"/>
     <col min="3" max="3" width="14.125" style="6" customWidth="1"/>
     <col min="4" max="4" width="47" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.75" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="6"/>
-    <col min="7" max="8" width="26.375" style="6" customWidth="1"/>
+    <col min="7" max="8" width="24.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="50.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.375" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1894,7 +2026,7 @@
         <v>43086</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>22</v>
@@ -1915,111 +2047,115 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="21">
+    <row r="5" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="49">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="50">
         <v>43086</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="51"/>
+      <c r="E5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="21">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
-        <v>43089</v>
-      </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="21">
+      <c r="C6" s="7">
+        <v>43091</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="26">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <v>43091</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="21">
+      <c r="H7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="2:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="17">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
-        <v>43091</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="C8" s="7">
+        <v>43102</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="66" x14ac:dyDescent="0.3">
       <c r="B9" s="21">
         <v>6</v>
       </c>
@@ -2028,25 +2164,25 @@
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>23</v>
+      <c r="G9" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="66" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="21">
         <v>7</v>
       </c>
@@ -2055,63 +2191,63 @@
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>85</v>
+      <c r="G10" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="I10" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="21">
+    </row>
+    <row r="11" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="26">
         <v>8</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="9">
         <v>43102</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>87</v>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="21">
+      <c r="B12" s="54">
         <v>9</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="24"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="21">
@@ -2153,7 +2289,9 @@
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
+      <c r="B16" s="21">
+        <v>13</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -2164,7 +2302,9 @@
       <c r="J16" s="24"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
+      <c r="B17" s="21">
+        <v>14</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -2175,7 +2315,9 @@
       <c r="J17" s="24"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
+      <c r="B18" s="21">
+        <v>15</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -2340,15 +2482,15 @@
       <c r="J32" s="24"/>
     </row>
     <row r="33" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="27"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>